<commit_message>
worked on colored rows
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Alle initiatieven" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Aangekondigd" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29,12 +30,15 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid"/>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -457,7 +462,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -482,7 +487,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -507,7 +512,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -532,7 +537,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -557,7 +562,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -582,7 +587,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -607,7 +612,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -632,7 +637,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -657,7 +662,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -682,7 +687,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -707,7 +712,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -732,7 +737,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -757,7 +762,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -782,7 +787,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -807,7 +812,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -832,7 +837,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -857,7 +862,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -882,7 +887,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -907,7 +912,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -932,24 +937,565 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Legislative proposal on multimodal digital mobility services</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-multimodal-digital-mobility-services</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Naam</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>URL</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>5G action plan</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-5g-action-plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Cybersecurity package</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-cyber-security-package</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Revision of airport charges</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-airport-charges</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Europe fit for the digital age strategy</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-digital-age-strategy</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Future of Research and Innovation and the European Research Area</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-european-research-area</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Horizon Europe research and innovation missions (non-legislative, Q4 2020)</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-horizon-europe-missions</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>A new industrial strategy</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-industrial-strategy</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>Digital Finance Strategy for the EU</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-fintech-action-plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>Revision of the provision of air services</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-air-services</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>A European Strategy for Data</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-european-data-strategy</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>Single Market Enforcement Action Plan</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-single-market-enforcement-action-plan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>Single Market Barriers Report</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-single-market-barriers-report</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>Small and medium-sized enterprises (SMEs) strategy</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-sme-strategy</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>Action plan on synergies between civil, defence and space industries</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-synergies-between-civil-defence-and-space-industries</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>Communication on Europe's digital decade: 2030 digital targets</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-europe-s-digital-decade-2030-digital-targets</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>Digital levy and a proposal for digital levy as own resource</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-digital-levy</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>Review of competition policy</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-review-of-competition-policy</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>Legislative proposal on computerised reservation systems (REFIT)</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>Legislative</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-computerised-reservation-systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>Renewed strategy for modern and safe retail payments</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>Niet-regelgevend</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-retail-digital-payments</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
         <is>
           <t>Legislative proposal on multimodal digital mobility services</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="C21" s="2" t="inlineStr">
         <is>
           <t>Legislative</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Aangekondigd</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>Aangekondigd</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
         <is>
           <t>https://www.europarl.europa.eu/legislative-train/theme-a-europe-fit-for-the-digital-age/file-multimodal-digital-mobility-services</t>
         </is>

</xml_diff>